<commit_message>
Updated Metadata and api status excel
</commit_message>
<xml_diff>
--- a/TF_UI_API_Intg_status.xlsx
+++ b/TF_UI_API_Intg_status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="217">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -701,6 +701,12 @@
   </si>
   <si>
     <t>Get Prod URL - parent grid</t>
+  </si>
+  <si>
+    <t>Garnishment Formula Overrides</t>
+  </si>
+  <si>
+    <t>Group Overrides</t>
   </si>
 </sst>
 </file>
@@ -757,7 +763,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -780,6 +786,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -907,7 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -984,6 +996,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2098,8 +2112,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:Q13" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:Q13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:Q14"/>
   <sortState ref="A2:J13">
     <sortCondition ref="A1:A13"/>
   </sortState>
@@ -2415,8 +2429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2785,99 +2799,100 @@
       <c r="P8" s="40"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="E9" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="41" t="s">
+      <c r="E9" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="G9" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" s="41" t="s">
+      <c r="G9" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="I9" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="41" t="s">
+      <c r="I9" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="K9" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="L9" s="41" t="s">
+      <c r="K9" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="M9" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="N9" s="41" t="s">
+      <c r="M9" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="N9" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="O9" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="P9" s="41"/>
+      <c r="O9" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="P9" s="40"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" t="s">
+      <c r="A10" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="41" t="s">
         <v>180</v>
       </c>
-      <c r="E10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G10" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="K10" t="s">
-        <v>66</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="K10" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="M10" t="s">
-        <v>66</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="M10" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="N10" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="O10" t="s">
-        <v>66</v>
-      </c>
+      <c r="O10" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="P10" s="41"/>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
@@ -4272,10 +4287,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4406,6 +4421,9 @@
       <c r="C3" t="s">
         <v>66</v>
       </c>
+      <c r="D3" t="s">
+        <v>111</v>
+      </c>
       <c r="E3" t="s">
         <v>211</v>
       </c>
@@ -4482,10 +4500,37 @@
         <v>194</v>
       </c>
     </row>
+    <row r="13" spans="1:17">
+      <c r="A13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>